<commit_message>
Test data update for Oncology pops
</commit_message>
<xml_diff>
--- a/Testdata/LIVEHTA_723_Data.xlsx
+++ b/Testdata/LIVEHTA_723_Data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VersionControl\pse.autotest\Testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E55B31C-A79D-4683-9F4D-601BF53D34DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10E9DCCE-FD52-4BA0-98FE-E911451C0D8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{EBA6B7B5-4164-47B4-905D-E5F060CAEA54}"/>
   </bookViews>
@@ -68,18 +68,6 @@
     <t>scenario2</t>
   </si>
   <si>
-    <t>ExcelReport-LIVEHTA_723 - Test723-Clinical-</t>
-  </si>
-  <si>
-    <t>WordReport-LIVEHTA_723 - Test723-Clinical-</t>
-  </si>
-  <si>
-    <t>LIVEHTA_723 - Test723</t>
-  </si>
-  <si>
-    <t>LIVEHTA_723 - Test723_radio_button</t>
-  </si>
-  <si>
     <t>Clinical</t>
   </si>
   <si>
@@ -113,7 +101,19 @@
     <t>\Testdata\Templates\SLRReport_SourceData\LIVEHTA_723_Testdata\ExpectedData_withFA13_and_FA19data.xlsx</t>
   </si>
   <si>
-    <t>LIVEHTA_723 - Test723 - 1/13/2023</t>
+    <t>NewImportLogic_3 - Test_Automation_3 - 1/13/2023</t>
+  </si>
+  <si>
+    <t>NewImportLogic_3 - Test_Automation_3</t>
+  </si>
+  <si>
+    <t>NewImportLogic_3 - Test_Automation_3_radio_button</t>
+  </si>
+  <si>
+    <t>ExcelReport-NewImportLogic_3 - Test_Automation_3-Clinical-</t>
+  </si>
+  <si>
+    <t>WordReport-NewImportLogic_3 - Test_Automation_3-Clinical-</t>
   </si>
 </sst>
 </file>
@@ -457,7 +457,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -467,8 +467,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7AC4BC85-93C4-414B-BB49-484C6267FF39}">
   <dimension ref="A1:J4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -489,7 +489,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -507,10 +507,10 @@
         <v>5</v>
       </c>
       <c r="H1" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="I1" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="J1" t="s">
         <v>6</v>
@@ -521,36 +521,36 @@
         <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H2" t="s">
         <v>12</v>
       </c>
-      <c r="D2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F2" t="s">
+      <c r="I2" t="s">
         <v>15</v>
       </c>
-      <c r="G2" t="s">
-        <v>23</v>
-      </c>
-      <c r="H2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I2" t="s">
-        <v>19</v>
-      </c>
       <c r="J2" t="s">
-        <v>10</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="J3" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
@@ -558,28 +558,28 @@
         <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="D4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4" t="s">
+        <v>20</v>
+      </c>
+      <c r="H4" t="s">
         <v>13</v>
       </c>
-      <c r="E4" t="s">
-        <v>14</v>
-      </c>
-      <c r="F4" t="s">
-        <v>15</v>
-      </c>
-      <c r="G4" t="s">
-        <v>24</v>
-      </c>
-      <c r="H4" t="s">
-        <v>17</v>
-      </c>
       <c r="I4" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="J4" t="s">
         <v>8</v>
@@ -587,5 +587,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
</xml_diff>